<commit_message>
fix write DID when data length is 5 byte and add color rule and width adapt
</commit_message>
<xml_diff>
--- a/DID_Status.xlsx
+++ b/DID_Status.xlsx
@@ -87,6 +87,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="0000FF00"/>
+          <bgColor rgb="0000FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FF0000"/>
+          <bgColor rgb="00FF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -433,6 +483,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="55" customWidth="1" min="3" max="3"/>
+    <col width="201" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -447,12 +503,12 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
           <t>Data</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Error</t>
         </is>
       </c>
     </row>
@@ -467,12 +523,11 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -485,12 +540,11 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -500,17 +554,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>KO</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>Negative response: Error code 0x14: Response too long</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="4">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="5">
+      <formula>"NOK"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -528,6 +589,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="67" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -537,17 +604,17 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
           <t>Data</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Error</t>
         </is>
       </c>
     </row>
@@ -559,17 +626,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Negative response: Error code 0x13: Invalid message length/format</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>0;0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Negative response: Error code 0x13: Invalid message length/format</t>
         </is>
       </c>
     </row>
@@ -581,21 +648,29 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Negative response: Error code 0x13: Invalid message length/format</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>0;0;0;0;1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>invalid index</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="4">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="5">
+      <formula>"NOK"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add file configuration and add CanApi4 support
</commit_message>
<xml_diff>
--- a/DID_Status.xlsx
+++ b/DID_Status.xlsx
@@ -2,33 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2610" yWindow="1995" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DID Read" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DID Write" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -42,27 +38,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -75,51 +56,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -137,7 +83,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -220,44 +166,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -284,15 +230,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -319,7 +264,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,142 +275,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -486,27 +454,27 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="55" customWidth="1" min="3" max="3"/>
-    <col width="201" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>DID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Resultat</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Error</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -520,12 +488,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00</t>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Time out No Response</t>
         </is>
       </c>
     </row>
@@ -537,12 +505,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00;0x80;0x00;0x05;0x00</t>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Time out No Response</t>
         </is>
       </c>
     </row>
@@ -559,16 +527,16 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Negative response: Error code 0x14: Response too long</t>
+          <t>Time out No Response</t>
         </is>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="4">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="2" operator="equal" dxfId="5">
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
       <formula>"NOK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -592,27 +560,27 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="67" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>DID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Error</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -631,7 +599,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Negative response: Error code 0x13: Invalid message length/format</t>
+          <t>Time out No Response</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -653,7 +621,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Negative response: Error code 0x13: Invalid message length/format</t>
+          <t>Time out No Response</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -664,10 +632,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="4">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="2" operator="equal" dxfId="5">
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
       <formula>"NOK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>